<commit_message>
Stori-006: Alias, Readme and Requeriments
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1102,6 +1102,156 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>¿cualés son las alianzas con comercios y proveedores de historiacard?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>HistoriaCard ha establecido alianzas con una amplia red de comercios y proveedores de servicios en todo México. Estas colaboraciones permiten a los usuarios de HistoriaCard disfrutar de descuentos exclusivos y promociones especiales. Este enfoque crea un ecosistema de valor añadido que beneficia tanto a los usuarios, al ofrecerles oportunidades de ahorro, como a los socios comerciales, al incrementar su visibilidad y atraer a más clientes.None</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>HistoriaCard ha forjado alianzas con una red extensa de comercios y proveedores de servicios en todo México. Estas alianzas permiten a los usuarios de
+HistoriaCard acceder a descuentos exclusivos y promociones especiales, creando un ecosistema de valor añadido que beneficia tanto a los usuarios como a los
+socios comerciales.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Alianzas con Comercios y Proveedores
+HistoriaCard ha forjado alianzas con una red extensa de comercios y proveedores de servicios en todo México. Estas alianzas permiten a los usuarios de
+HistoriaCard acceder a descuentos exclusivos y promociones especiales, creando un ecosistema de valor añadido que beneficia tanto a los usuarios como a los</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Alianzas con Comercios y Proveedores
+HistoriaCard ha forjado alianzas con una red extensa de comercios y proveedores de servicios en todo México. Estas alianzas permiten a los usuarios de
+HistoriaCard acceder a descuentos exclusivos y promociones especiales, creando un ecosistema de valor añadido que beneficia tanto a los usuarios como a los
+socios comerciales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>¿qué se puede hacer en la sección de mi perfil de la app de hihistoriacardacard?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>En la sección de "Mi Perfil" de la app de HistoriaCard, los usuarios pueden realizar diversas configuraciones para personalizar su experiencia. Algunas de las funcionalidades incluyen:
+1. **Configuración de Notificaciones**: Los usuarios pueden elegir qué tipos de alertas y notificaciones desean recibir, como avisos de saldo bajo, recordatorios de pago y alertas de transacciones inusuales.
+2. **Cambio de Idioma**: La app permite cambiar el idioma entre español e inglés, adaptándose a las preferencias del usuario.
+3. **Personalización de Seguridad**: Los usuarios pueden ajustar configuraciones relacionadas con la seguridad de su cuenta, asegurando que la app se adapte a sus necesidades.
+Esta sección está diseñada para ofrecer un mayor control y comodidad a los usuarios de HistoriaCard.None</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>8. Configuración
+La sección de Configuración permite a los usuarios personalizar la app de acuerdo con sus preferencias y necesidades de seguridad.
+Notificaciones: Configura qué tipos de alertas y notificaciones deseas recibir, como avisos de saldo bajo, recordatorios de pago, o alertas de transacciones
+inusuales.
+Idioma: Cambia el idioma de la app entre español e inglés, adaptándose a las preferencias del usuario.</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>8. Configuración
+La sección de Configuración permite a los usuarios personalizar la app de acuerdo con sus preferencias y necesidades de seguridad.
+Notificaciones: Configura qué tipos de alertas y notificaciones deseas recibir, como avisos de saldo bajo, recordatorios de pago, o alertas de transacciones</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>8. Configuración
+La sección de Configuración permite a los usuarios personalizar la app de acuerdo con sus preferencias y necesidades de seguridad.
+Notificaciones: Configura qué tipos de alertas y notificaciones deseas recibir, como avisos de saldo bajo, recordatorios de pago, o alertas de transacciones
+inusuales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ¿es posible acceder usando mi huella digital a mi app de historiacard?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Sí, es posible acceder a tu app de HistoriaCard utilizando tu huella digital. La aplicación cuenta con autenticación biométrica, lo que permite a los usuarios acceder a su cuenta mediante huella digital o reconocimiento facial. Esto garantiza que solo el titular de la cuenta pueda acceder a la misma, protegiendo así la información y los fondos de los usuarios.None</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>proteger la información y los fondos de sus usuarios.
+Cifrado de extremo a extremo: Toda la comunicación dentro de la app está cifrada, asegurando que los datos sensibles nunca sean vulnerables a
+intercepciones.
+Autenticación biométrica: Los usuarios pueden acceder a su cuenta mediante huella digital o reconocimiento facial, garantizando que solo el titular de la
+cuenta pueda acceder a la misma.</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>directamente desde la notificación.
+Actualizaciones constantes: La app se actualiza regularmente para incorporar las últimas mejoras en seguridad y tecnología, manteniendo la protección de
+los usuarios a la vanguardia.</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>forma independiente.
+Solicitudes de soporte: Los usuarios pueden abrir tickets de soporte para problemas más complejos y hacer un seguimiento de su estado directamente desde
+la app.
+Llamadas de emergencia: En situaciones de urgencia, como el robo o pérdida de la tarjeta, los usuarios pueden solicitar una llamada inmediata de un agente
+de soporte para tomar medidas rápidas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>¿cuál es la visión de hihistoriacardacard?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>La visión de HistoriaCard es ofrecer una experiencia bancaria completa, segura y sin complicaciones, tanto a través de su tarjeta de débito como de su tarjeta de crédito. La tarjeta de débito está diseñada para aquellos que prefieren manejar sus finanzas sin crédito, facilitando una gestión efectiva de su dinero. Por otro lado, la tarjeta de crédito busca ayudar a los usuarios a construir o mejorar su historial crediticio, educándolos sobre el manejo responsable del crédito, lo cual es fundamental para alcanzar la estabilidad financiera. En resumen, HistoriaCard se enfoca en empoderar a sus usuarios en la gestión de sus finanzas de manera segura y accesible.None</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Tarjeta de Débito HistoriaCard
+La tarjeta de débito HistoriaCard ofrece una experiencia bancaria completa, segura y sin complicaciones. Es ideal para aquellos que prefieren manejar sus finanzas
+sin crédito, permitiendo una gestión fácil y efectiva de su dinero.
+Características principales:
+Costo de emisión: Gratuito al abrir una cuenta en la app de HistoriaCard, con la tarjeta enviada directamente al domicilio del usuario.</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Tarjeta de Débito HistoriaCard
+La tarjeta de débito HistoriaCard ofrece una experiencia bancaria completa, segura y sin complicaciones. Es ideal para aquellos que prefieren manejar sus finanzas
+sin crédito, permitiendo una gestión fácil y efectiva de su dinero.</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Tarjeta de Crédito HistoriaCard
+La tarjeta de crédito HistoriaCard es un producto clave para aquellos que buscan construir o mejorar su historial crediticio. Esta tarjeta no solo permite realizar
+compras, sino que también educa a los usuarios sobre el manejo responsable del crédito, un componente esencial para alcanzar la estabilidad financiera.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>